<commit_message>
Major Grade and DB Update
Major Grade and DB Update
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Students Database.xlsx
+++ b/Batch 2018-20/Sem 1/Students Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUOBHAM MURUDKAR\Desktop\SIMSR-Results-Generator-master\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0157E3D-5D8C-4A9C-A984-9589F57F711C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5996C1-F432-4602-865A-021C64E72B3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AFC29160-401D-4461-8898-326E7690AE3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AFC29160-401D-4461-8898-326E7690AE3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6662,6 +6662,56 @@
         <a:xfrm>
           <a:off x="3230032" y="79673450"/>
           <a:ext cx="626536" cy="873125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8288</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>885825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AFB76BA-C41F-4A16-A2CE-8E70729772F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId117" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4086225" y="24212550"/>
+          <a:ext cx="694088" cy="885825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6972,7 +7022,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5826A716-B557-4E76-9620-9E98F48B9924}">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>